<commit_message>
updated bom with digireel
impulse rev c
</commit_message>
<xml_diff>
--- a/hardware/impulse/rev_c/impulse_bom.xlsx
+++ b/hardware/impulse/rev_c/impulse_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="144">
   <si>
     <t>Qty</t>
   </si>
@@ -38,6 +38,9 @@
     <t>DIGIKEY</t>
   </si>
   <si>
+    <t>DIGIREEL</t>
+  </si>
+  <si>
     <t>MOUSER</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
     <t>WM4893CT-ND</t>
   </si>
   <si>
+    <t>WM4893DKR-ND</t>
+  </si>
+  <si>
     <t>BD2425N50200A</t>
   </si>
   <si>
@@ -65,6 +71,9 @@
     <t>1173-1063-1-ND</t>
   </si>
   <si>
+    <t>1173-1063-6-ND</t>
+  </si>
+  <si>
     <t>12pF</t>
   </si>
   <si>
@@ -83,6 +92,9 @@
     <t>712-1257-1-ND</t>
   </si>
   <si>
+    <t>712-1257-6-ND</t>
+  </si>
+  <si>
     <t>22pF</t>
   </si>
   <si>
@@ -92,6 +104,9 @@
     <t>445-1239-1-ND</t>
   </si>
   <si>
+    <t>445-1239-6-ND</t>
+  </si>
+  <si>
     <t>68pF</t>
   </si>
   <si>
@@ -101,6 +116,9 @@
     <t>445-1245-1-ND</t>
   </si>
   <si>
+    <t>445-1245-6-ND</t>
+  </si>
+  <si>
     <t>0.01uF</t>
   </si>
   <si>
@@ -110,6 +128,9 @@
     <t>445-1260-1-ND</t>
   </si>
   <si>
+    <t>445-1260-6-ND</t>
+  </si>
+  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -119,6 +140,9 @@
     <t>445-1265-1-ND</t>
   </si>
   <si>
+    <t>445-1265-6-ND</t>
+  </si>
+  <si>
     <t>2.2uF</t>
   </si>
   <si>
@@ -128,6 +152,9 @@
     <t>445-3882-1-ND</t>
   </si>
   <si>
+    <t>445-3882-6-ND</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -146,13 +173,19 @@
     <t>478-2561-1-ND</t>
   </si>
   <si>
+    <t>478-2561-6-ND</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
     <t>LED-0603</t>
   </si>
   <si>
     <t>D1, D2</t>
   </si>
   <si>
-    <t>LED</t>
+    <t>LED – BLUE</t>
   </si>
   <si>
     <t>IMPULSE_GECKO_HEADER</t>
@@ -188,6 +221,9 @@
     <t>712-1419-1-ND</t>
   </si>
   <si>
+    <t>712-1419-6-ND</t>
+  </si>
+  <si>
     <t>MOSFET-NCHANNELXFDN-3</t>
   </si>
   <si>
@@ -203,6 +239,9 @@
     <t>DMN2400UFB4-7DICT-ND</t>
   </si>
   <si>
+    <t>DMN2400UFB4-7DIDKR-ND</t>
+  </si>
+  <si>
     <t>RESISTOR</t>
   </si>
   <si>
@@ -218,9 +257,15 @@
     <t>RHM2.2CECT-ND</t>
   </si>
   <si>
+    <t>RHM2.2CEDKR-ND</t>
+  </si>
+  <si>
     <t>R2, R16</t>
   </si>
   <si>
+    <t>RHM470BHDKR-ND</t>
+  </si>
+  <si>
     <t>2.2k</t>
   </si>
   <si>
@@ -230,6 +275,9 @@
     <t>RHM2.2KCECT-ND</t>
   </si>
   <si>
+    <t>RHM2.2KCEDKR-ND</t>
+  </si>
+  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -239,6 +287,9 @@
     <t>RHM4.7KCECT-ND</t>
   </si>
   <si>
+    <t>RHM4.7KCEDKR-ND</t>
+  </si>
+  <si>
     <t>43k</t>
   </si>
   <si>
@@ -248,6 +299,9 @@
     <t>RHM43KCECT-ND</t>
   </si>
   <si>
+    <t>RHM43KCEDKR-ND</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
@@ -257,6 +311,9 @@
     <t>RHM100KCECT-ND</t>
   </si>
   <si>
+    <t>RHM100KCEDKR-ND</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
@@ -266,6 +323,9 @@
     <t>RHM1.0MCECT-ND</t>
   </si>
   <si>
+    <t>RHM1.0MCEDKR-ND</t>
+  </si>
+  <si>
     <t>4.7M</t>
   </si>
   <si>
@@ -275,6 +335,9 @@
     <t>541-4.7MJCT-ND</t>
   </si>
   <si>
+    <t>541-4.7MJDKR-ND</t>
+  </si>
+  <si>
     <t>5.1M</t>
   </si>
   <si>
@@ -284,6 +347,9 @@
     <t>RHM5.1MBICT-ND</t>
   </si>
   <si>
+    <t>RHM5.1MBIDKR-ND</t>
+  </si>
+  <si>
     <t>DS2411</t>
   </si>
   <si>
@@ -299,6 +365,9 @@
     <t>DS2411R+CT-ND</t>
   </si>
   <si>
+    <t>DS2411R+DKR-ND</t>
+  </si>
+  <si>
     <t>FM25LBTDFN-8</t>
   </si>
   <si>
@@ -329,6 +398,9 @@
     <t>296-18102-1-ND</t>
   </si>
   <si>
+    <t>296-18102-6-ND</t>
+  </si>
+  <si>
     <t>CC2420RGZ</t>
   </si>
   <si>
@@ -344,6 +416,9 @@
     <t>296-19585-1-ND</t>
   </si>
   <si>
+    <t>296-19585-6-ND</t>
+  </si>
+  <si>
     <t>TXC-7V</t>
   </si>
   <si>
@@ -353,6 +428,9 @@
     <t>887-1799-1-ND</t>
   </si>
   <si>
+    <t>887-1799-6-ND</t>
+  </si>
+  <si>
     <t>ABRACON-ABS05</t>
   </si>
   <si>
@@ -366,6 +444,9 @@
   </si>
   <si>
     <t>535-11899-1-ND</t>
+  </si>
+  <si>
+    <t>535-11899-6-ND</t>
   </si>
 </sst>
 </file>
@@ -463,16 +544,16 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -492,13 +573,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E16" activeCellId="0" pane="topLeft" sqref="E16"/>
+      <selection activeCell="F25" activeCellId="0" pane="topLeft" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.1938775510204"/>
@@ -506,9 +587,10 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.5561224489796"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.9183673469388"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.219387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -539,25 +621,31 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -565,19 +653,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -585,22 +676,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -608,22 +702,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -631,22 +728,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -654,22 +754,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -677,22 +780,25 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -700,22 +806,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -723,39 +832,45 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
@@ -763,19 +878,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
@@ -783,22 +898,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -806,19 +921,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -826,65 +944,74 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>2.2</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>470</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -892,22 +1019,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>70</v>
+        <v>85</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
@@ -915,22 +1045,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
@@ -938,22 +1071,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>76</v>
+        <v>93</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
@@ -961,22 +1097,25 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E21" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G21" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
@@ -984,22 +1123,25 @@
         <v>4</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>82</v>
+        <v>101</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
@@ -1007,22 +1149,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
@@ -1030,22 +1175,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
@@ -1053,22 +1201,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
@@ -1076,25 +1227,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>99</v>
+        <v>121</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
@@ -1102,19 +1253,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>103</v>
+        <v>126</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
@@ -1122,22 +1276,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>108</v>
+        <v>132</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
@@ -1145,19 +1302,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>111</v>
+        <v>136</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -1165,22 +1325,25 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>116</v>
+        <v>140</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>